<commit_message>
escalas começando dia 1
</commit_message>
<xml_diff>
--- a/planilha/dezembro/Escala ASO1 - Calafate - 1° Turno - Dezembro.xlsx
+++ b/planilha/dezembro/Escala ASO1 - Calafate - 1° Turno - Dezembro.xlsx
@@ -28,12 +28,12 @@
     <t>Ps</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -103,7 +103,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>25/11/19</t>
+    <t>29/11/19</t>
   </si>
 </sst>
 </file>
@@ -162,10 +162,10 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -556,92 +556,98 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="O2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="Q2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="R2" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="S2" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="T2" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="O2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="P2" s="1" t="n">
+      <c r="U2" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="W2" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="X2" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="Y2" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="Z2" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="AA2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="V2" s="1" t="n">
+      <c r="AB2" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="W2" s="1" t="n">
+      <c r="AC2" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="X2" s="1" t="n">
+      <c r="AD2" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="AE2" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="AF2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="AA2" s="1" t="n">
+      <c r="AG2" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="AB2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE2" s="1" t="n"/>
-      <c r="AF2" s="1" t="n"/>
-      <c r="AG2" s="1" t="n"/>
       <c r="AH2" s="1" t="n"/>
       <c r="AI2" s="1" t="n"/>
       <c r="AJ2" s="1" t="n"/>
@@ -659,19 +665,19 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>3</v>
@@ -680,19 +686,19 @@
         <v>4</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>3</v>
@@ -701,19 +707,19 @@
         <v>4</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>3</v>
@@ -722,23 +728,29 @@
         <v>4</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AD3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AE3" s="1" t="n"/>
-      <c r="AF3" s="1" t="n"/>
-      <c r="AG3" s="1" t="n"/>
+      <c r="AF3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AH3" s="1" t="n"/>
       <c r="AI3" s="1" t="n"/>
       <c r="AJ3" s="1" t="n"/>
@@ -782,96 +794,102 @@
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE4" s="4" t="n"/>
-      <c r="AF4" s="4" t="n"/>
-      <c r="AG4" s="4" t="n"/>
-      <c r="AH4" s="4" t="n"/>
-      <c r="AI4" s="4" t="n"/>
-      <c r="AJ4" s="4" t="n"/>
-      <c r="AK4" s="4" t="n"/>
+        <v>8</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH4" s="3" t="n"/>
+      <c r="AI4" s="3" t="n"/>
+      <c r="AJ4" s="3" t="n"/>
+      <c r="AK4" s="3" t="n"/>
       <c r="AM4">
         <f>COUNTIF(B4:AG4; "B1")</f>
         <v/>
@@ -920,13 +938,13 @@
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -936,16 +954,16 @@
         <v>13</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>8</v>
@@ -953,60 +971,66 @@
       <c r="M5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>7</v>
+      <c r="T5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE5" s="5" t="n"/>
-      <c r="AF5" s="5" t="n"/>
-      <c r="AG5" s="5" t="n"/>
+        <v>8</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="AH5" s="5" t="n"/>
       <c r="AI5" s="5" t="n"/>
       <c r="AJ5" s="5" t="n"/>
@@ -1060,96 +1084,102 @@
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE6" s="4" t="n"/>
-      <c r="AF6" s="4" t="n"/>
-      <c r="AG6" s="4" t="n"/>
-      <c r="AH6" s="4" t="n"/>
-      <c r="AI6" s="4" t="n"/>
-      <c r="AJ6" s="4" t="n"/>
-      <c r="AK6" s="4" t="n"/>
+        <v>19</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH6" s="3" t="n"/>
+      <c r="AI6" s="3" t="n"/>
+      <c r="AJ6" s="3" t="n"/>
+      <c r="AK6" s="3" t="n"/>
       <c r="AM6">
         <f>COUNTIF(B6:AG6; "B1")</f>
         <v/>
@@ -1198,77 +1228,79 @@
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>7</v>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s"/>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="5" t="s"/>
+      <c r="H7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="5" t="s"/>
-      <c r="K7" s="5" t="s"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L7" s="5" t="s"/>
-      <c r="M7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>7</v>
+      <c r="M7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P7" s="5" t="s"/>
-      <c r="Q7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="3" t="s">
+      <c r="Q7" s="5" t="s"/>
+      <c r="R7" s="5" t="s"/>
+      <c r="S7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="U7" s="5" t="s"/>
+        <v>13</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="V7" s="5" t="s"/>
-      <c r="W7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>13</v>
+      <c r="W7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AA7" s="5" t="s"/>
-      <c r="AB7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AB7" s="5" t="s"/>
+      <c r="AC7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE7" s="5" t="n"/>
-      <c r="AF7" s="5" t="n"/>
-      <c r="AG7" s="5" t="n"/>
+        <v>7</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG7" s="5" t="s"/>
       <c r="AH7" s="5" t="n"/>
       <c r="AI7" s="5" t="n"/>
       <c r="AJ7" s="5" t="n"/>
@@ -1322,80 +1354,82 @@
         <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s"/>
-      <c r="G8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="4" t="s"/>
-      <c r="K8" s="4" t="s"/>
-      <c r="L8" s="4" t="s"/>
-      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s"/>
+      <c r="G8" s="3" t="s"/>
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="3" t="s"/>
+      <c r="M8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P8" s="4" t="s"/>
-      <c r="Q8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="4" t="s"/>
-      <c r="V8" s="4" t="s"/>
-      <c r="W8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="3" t="s"/>
+      <c r="Q8" s="3" t="s"/>
+      <c r="R8" s="3" t="s"/>
+      <c r="S8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" s="3" t="s"/>
+      <c r="W8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="4" t="s"/>
-      <c r="AB8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE8" s="4" t="n"/>
-      <c r="AF8" s="4" t="n"/>
-      <c r="AG8" s="4" t="n"/>
-      <c r="AH8" s="4" t="n"/>
-      <c r="AI8" s="4" t="n"/>
-      <c r="AJ8" s="4" t="n"/>
-      <c r="AK8" s="4" t="n"/>
+        <v>19</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="3" t="s"/>
+      <c r="AB8" s="3" t="s"/>
+      <c r="AC8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG8" s="3" t="s"/>
+      <c r="AH8" s="3" t="n"/>
+      <c r="AI8" s="3" t="n"/>
+      <c r="AJ8" s="3" t="n"/>
+      <c r="AK8" s="3" t="n"/>
       <c r="AM8">
         <f>COUNTIF(B8:AG8; "B1")</f>
         <v/>
@@ -1444,75 +1478,79 @@
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s"/>
-      <c r="F9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="5" t="s"/>
+      <c r="G9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="5" t="s"/>
-      <c r="J9" s="5" t="s"/>
+        <v>8</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K9" s="5" t="s"/>
-      <c r="L9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>7</v>
+      <c r="L9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="O9" s="5" t="s"/>
-      <c r="P9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R9" s="3" t="s">
+      <c r="P9" s="5" t="s"/>
+      <c r="Q9" s="5" t="s"/>
+      <c r="R9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T9" s="5" t="s"/>
+      <c r="T9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="U9" s="5" t="s"/>
-      <c r="V9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>13</v>
+      <c r="V9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Z9" s="5" t="s"/>
-      <c r="AA9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB9" s="3" t="s">
+      <c r="AA9" s="5" t="s"/>
+      <c r="AB9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AC9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD9" s="5" t="s"/>
-      <c r="AE9" s="5" t="n"/>
-      <c r="AF9" s="5" t="n"/>
-      <c r="AG9" s="5" t="n"/>
+        <v>7</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF9" s="5" t="s"/>
+      <c r="AG9" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="AH9" s="5" t="n"/>
       <c r="AI9" s="5" t="n"/>
       <c r="AJ9" s="5" t="n"/>

</xml_diff>